<commit_message>
fixed accuracy confidence interval calc file xlsx
</commit_message>
<xml_diff>
--- a/ACCURACY CONFIDENCE INTERVAL - Calculation.xlsx
+++ b/ACCURACY CONFIDENCE INTERVAL - Calculation.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Google Drive\Work\Master Data Science - Bologna Business School\2021\Extra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nik\BBS-TextMining\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BD4412D9-E6B4-42BB-BB0F-5703703C7742}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCD3B1C-ADEE-4B3D-BCE1-A6F4B1C80D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -300,13 +300,13 @@
     <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -527,8 +527,8 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
@@ -542,16 +542,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" ht="14.25">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:8">
+    <row r="3" spans="1:8" ht="12.75">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:8">
+    <row r="4" spans="1:8" ht="12.75">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -559,7 +559,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:8">
+    <row r="5" spans="1:8" ht="12.75">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -567,7 +567,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:8">
+    <row r="6" spans="1:8" ht="12.75">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -575,7 +575,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:8">
+    <row r="7" spans="1:8" ht="12.75">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -585,7 +585,7 @@
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:8">
+    <row r="8" spans="1:8" ht="12.75">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -614,7 +614,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8">
+    <row r="9" spans="1:8" ht="12.75">
       <c r="B9" s="11"/>
       <c r="C9" s="11">
         <f>2 * (B6 + B7^2)</f>
@@ -632,12 +632,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8">
+    <row r="12" spans="1:8" ht="12.75">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8">
+    <row r="13" spans="1:8" ht="12.75">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -645,7 +645,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="14" spans="1:8">
+    <row r="14" spans="1:8" ht="12.75">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -654,11 +654,11 @@
         <v>1.9599639845400536</v>
       </c>
     </row>
-    <row r="15" spans="1:8">
+    <row r="15" spans="1:8" ht="12.75">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:8">
+    <row r="16" spans="1:8" ht="12.75">
       <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
@@ -666,7 +666,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" ht="12.75">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -677,7 +677,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" ht="12.75">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -688,31 +688,31 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" ht="12.75">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B19" s="29">
+      <c r="B19" s="32">
         <f>( B17*(1-B17) / B18 ) + ( C17 * (1-C17) / C18)</f>
         <v>4.2875000000000005E-3</v>
       </c>
       <c r="C19" s="30"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" ht="12.75">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B20" s="31">
+      <c r="B20" s="29">
         <f>ABS(C17 - B17)</f>
         <v>0.1</v>
       </c>
       <c r="C20" s="30"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" ht="12.75">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B21" s="31">
+      <c r="B21" s="29">
         <f>B20</f>
         <v>0.1</v>
       </c>
@@ -735,7 +735,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" ht="12.75">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -751,8 +751,8 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:8">
-      <c r="A23" s="32" t="str">
+    <row r="23" spans="1:8" ht="12.75">
+      <c r="A23" s="33" t="str">
         <f>IF(AND(F21&gt;=0,F22&lt;=0), "Zero is contained in the interval so the difference is not statistically significant", "Zero is no contained in the interval so the difference is statistically significant")</f>
         <v>Zero is contained in the interval so the difference is not statistically significant</v>
       </c>
@@ -764,12 +764,12 @@
       <c r="G23" s="30"/>
       <c r="H23" s="30"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" ht="12.75">
       <c r="A26" s="3" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" ht="12.75">
       <c r="A27" s="4" t="s">
         <v>2</v>
       </c>
@@ -777,7 +777,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" ht="12.75">
       <c r="A28" s="4" t="s">
         <v>5</v>
       </c>
@@ -786,11 +786,11 @@
         <v>1.9599639845400536</v>
       </c>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" ht="12.75">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" ht="12.75">
       <c r="B30" s="13" t="s">
         <v>14</v>
       </c>
@@ -798,7 +798,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" ht="12.75">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
@@ -809,7 +809,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" ht="12.75">
       <c r="A32" s="4" t="s">
         <v>4</v>
       </c>
@@ -820,32 +820,32 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" ht="12.75">
       <c r="A33" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B33" s="29">
+      <c r="B33" s="32">
         <f>( B31*(1-B31) / B32 ) + ( C31 * (1-C31) / C32)</f>
         <v>4.2875000000000005E-3</v>
       </c>
       <c r="C33" s="30"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" ht="12.75">
       <c r="A34" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B34" s="31">
+      <c r="B34" s="29">
         <f>ABS(C31 - B31)</f>
         <v>0.1</v>
       </c>
       <c r="C34" s="30"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" ht="12.75">
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" ht="14.25">
       <c r="A36" s="4" t="s">
         <v>24</v>
       </c>
@@ -861,11 +861,11 @@
         <v>1.5272070966424252</v>
       </c>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" ht="12.75">
       <c r="A37" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B37" s="33">
+      <c r="B37" s="31">
         <f>D36</f>
         <v>1.5272070966424252</v>
       </c>
@@ -996,8 +996,8 @@
     </row>
     <row r="49" spans="1:1" ht="12.75">
       <c r="A49" s="27" t="str">
-        <f>IF(AND(F47&gt;=0,F48&lt;=0), "Zero is contained in the interval so the difference is statistically significant", "Zero is no longer contained in the interval so the difference is not statistically significant")</f>
-        <v>Zero is no longer contained in the interval so the difference is not statistically significant</v>
+        <f>IF(AND(F47&gt;=0,F48&lt;=0), "Zero is contained in the interval so the difference is statistically significant", "Zero is no longer contained in the interval so the difference is statistically significant")</f>
+        <v>Zero is no longer contained in the interval so the difference is statistically significant</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="12.75">

</xml_diff>

<commit_message>
fixed errors in ACCURACY CONFIDENCE INTERVAL - Calculation.xlsx
</commit_message>
<xml_diff>
--- a/ACCURACY CONFIDENCE INTERVAL - Calculation.xlsx
+++ b/ACCURACY CONFIDENCE INTERVAL - Calculation.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nik\BBS-TextMining\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nicola.piscaglia\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7FCD3B1C-ADEE-4B3D-BCE1-A6F4B1C80D29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8183117A-4996-4B3B-8B35-D544424DF5EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="57480" yWindow="10605" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Accuracy Confidence Interval" sheetId="1" r:id="rId1"/>
@@ -252,7 +252,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -307,6 +307,9 @@
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normale" xfId="0" builtinId="0"/>
@@ -527,14 +530,14 @@
   </sheetPr>
   <dimension ref="A1:H53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A50" sqref="A50"/>
+    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23:H23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="93.42578125" customWidth="1"/>
-    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="1" max="1" width="93.44140625" customWidth="1"/>
+    <col min="2" max="2" width="19.71875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" customHeight="1">
@@ -542,16 +545,16 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="14.25">
+    <row r="2" spans="1:8" ht="13.8">
       <c r="B2" s="2"/>
     </row>
-    <row r="3" spans="1:8" ht="12.75">
+    <row r="3" spans="1:8" ht="12.3">
       <c r="A3" s="3" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
     </row>
-    <row r="4" spans="1:8" ht="12.75">
+    <row r="4" spans="1:8" ht="12.3">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -559,7 +562,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.75">
+    <row r="5" spans="1:8" ht="12.3">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -567,7 +570,7 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.75">
+    <row r="6" spans="1:8" ht="12.3">
       <c r="A6" s="4" t="s">
         <v>4</v>
       </c>
@@ -575,7 +578,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.75">
+    <row r="7" spans="1:8" ht="12.3">
       <c r="A7" s="4" t="s">
         <v>5</v>
       </c>
@@ -585,7 +588,7 @@
       </c>
       <c r="C7" s="6"/>
     </row>
-    <row r="8" spans="1:8" ht="12.75">
+    <row r="8" spans="1:8" ht="12.3">
       <c r="A8" s="4" t="s">
         <v>6</v>
       </c>
@@ -614,7 +617,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="12.75">
+    <row r="9" spans="1:8" ht="12.3">
       <c r="B9" s="11"/>
       <c r="C9" s="11">
         <f>2 * (B6 + B7^2)</f>
@@ -632,12 +635,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="12.75">
+    <row r="12" spans="1:8" ht="12.3">
       <c r="A12" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="12.75">
+    <row r="13" spans="1:8" ht="12.3">
       <c r="A13" s="4" t="s">
         <v>2</v>
       </c>
@@ -645,7 +648,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="12.75">
+    <row r="14" spans="1:8" ht="12.3">
       <c r="A14" s="4" t="s">
         <v>5</v>
       </c>
@@ -654,11 +657,11 @@
         <v>1.9599639845400536</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="12.75">
+    <row r="15" spans="1:8" ht="12.3">
       <c r="B15" s="4"/>
       <c r="C15" s="4"/>
     </row>
-    <row r="16" spans="1:8" ht="12.75">
+    <row r="16" spans="1:8" ht="12.6">
       <c r="B16" s="13" t="s">
         <v>14</v>
       </c>
@@ -666,7 +669,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="12.75">
+    <row r="17" spans="1:8" ht="12.3">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
@@ -677,7 +680,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.75">
+    <row r="18" spans="1:8" ht="12.3">
       <c r="A18" s="4" t="s">
         <v>4</v>
       </c>
@@ -688,7 +691,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="12.75">
+    <row r="19" spans="1:8" ht="12.3">
       <c r="A19" s="4" t="s">
         <v>17</v>
       </c>
@@ -698,7 +701,7 @@
       </c>
       <c r="C19" s="30"/>
     </row>
-    <row r="20" spans="1:8" ht="12.75">
+    <row r="20" spans="1:8" ht="12.3">
       <c r="A20" s="4" t="s">
         <v>18</v>
       </c>
@@ -708,7 +711,7 @@
       </c>
       <c r="C20" s="30"/>
     </row>
-    <row r="21" spans="1:8" ht="12.75">
+    <row r="21" spans="1:8" ht="12.3">
       <c r="A21" s="4" t="s">
         <v>19</v>
       </c>
@@ -735,7 +738,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="12.75">
+    <row r="22" spans="1:8" ht="12.3">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -751,9 +754,9 @@
         <v>22</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="12.75">
+    <row r="23" spans="1:8" ht="12.3">
       <c r="A23" s="33" t="str">
-        <f>IF(AND(F21&gt;=0,F22&lt;=0), "Zero is contained in the interval so the difference is not statistically significant", "Zero is no contained in the interval so the difference is statistically significant")</f>
+        <f>IF(AND(G21&gt;=0,G22&lt;=0), "Zero is contained in the interval so the difference is not statistically significant", "Zero is no contained in the interval so the difference is statistically significant")</f>
         <v>Zero is contained in the interval so the difference is not statistically significant</v>
       </c>
       <c r="B23" s="30"/>
@@ -764,12 +767,12 @@
       <c r="G23" s="30"/>
       <c r="H23" s="30"/>
     </row>
-    <row r="26" spans="1:8" ht="12.75">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:8" ht="24.6">
+      <c r="A26" s="34" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="12.75">
+    <row r="27" spans="1:8" ht="12.3">
       <c r="A27" s="4" t="s">
         <v>2</v>
       </c>
@@ -777,7 +780,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="12.75">
+    <row r="28" spans="1:8" ht="12.3">
       <c r="A28" s="4" t="s">
         <v>5</v>
       </c>
@@ -786,11 +789,11 @@
         <v>1.9599639845400536</v>
       </c>
     </row>
-    <row r="29" spans="1:8" ht="12.75">
+    <row r="29" spans="1:8" ht="12.3">
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
     </row>
-    <row r="30" spans="1:8" ht="12.75">
+    <row r="30" spans="1:8" ht="12.6">
       <c r="B30" s="13" t="s">
         <v>14</v>
       </c>
@@ -798,7 +801,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="31" spans="1:8" ht="12.75">
+    <row r="31" spans="1:8" ht="12.3">
       <c r="A31" s="4" t="s">
         <v>16</v>
       </c>
@@ -809,7 +812,7 @@
         <v>0.25</v>
       </c>
     </row>
-    <row r="32" spans="1:8" ht="12.75">
+    <row r="32" spans="1:8" ht="12.3">
       <c r="A32" s="4" t="s">
         <v>4</v>
       </c>
@@ -820,7 +823,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="12.75">
+    <row r="33" spans="1:8" ht="12.3">
       <c r="A33" s="4" t="s">
         <v>17</v>
       </c>
@@ -830,7 +833,7 @@
       </c>
       <c r="C33" s="30"/>
     </row>
-    <row r="34" spans="1:8" ht="12.75">
+    <row r="34" spans="1:8" ht="12.3">
       <c r="A34" s="4" t="s">
         <v>18</v>
       </c>
@@ -840,12 +843,12 @@
       </c>
       <c r="C34" s="30"/>
     </row>
-    <row r="35" spans="1:8" ht="12.75">
+    <row r="35" spans="1:8" ht="12.3">
       <c r="B35" s="30"/>
       <c r="C35" s="30"/>
       <c r="E35" s="15"/>
     </row>
-    <row r="36" spans="1:8" ht="14.25">
+    <row r="36" spans="1:8" ht="13.8">
       <c r="A36" s="4" t="s">
         <v>24</v>
       </c>
@@ -861,7 +864,7 @@
         <v>1.5272070966424252</v>
       </c>
     </row>
-    <row r="37" spans="1:8" ht="12.75">
+    <row r="37" spans="1:8" ht="12.3">
       <c r="A37" s="18" t="s">
         <v>26</v>
       </c>
@@ -876,7 +879,7 @@
       <c r="G37" s="19"/>
       <c r="H37" s="19"/>
     </row>
-    <row r="38" spans="1:8" ht="12.75">
+    <row r="38" spans="1:8" ht="12.3">
       <c r="A38" s="20" t="s">
         <v>27</v>
       </c>
@@ -885,11 +888,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="39" spans="1:8" ht="12.75">
+    <row r="39" spans="1:8" ht="12.3">
       <c r="A39" s="4"/>
       <c r="B39" s="22"/>
     </row>
-    <row r="40" spans="1:8" ht="12.75">
+    <row r="40" spans="1:8" ht="12.3">
       <c r="A40" s="4" t="s">
         <v>28</v>
       </c>
@@ -898,7 +901,7 @@
         <v>0.12429229230192552</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="12.75">
+    <row r="41" spans="1:8" ht="12.3">
       <c r="A41" s="23" t="s">
         <v>29</v>
       </c>
@@ -907,14 +910,14 @@
         <v>0.87570770769807449</v>
       </c>
     </row>
-    <row r="42" spans="1:8" ht="12.75">
+    <row r="42" spans="1:8" ht="12.3">
       <c r="A42" s="4"/>
       <c r="C42" s="25"/>
       <c r="D42" s="26"/>
       <c r="E42" s="25"/>
       <c r="G42" s="4"/>
     </row>
-    <row r="43" spans="1:8" ht="12.75">
+    <row r="43" spans="1:8" ht="12.3">
       <c r="A43" s="4" t="s">
         <v>30</v>
       </c>
@@ -940,7 +943,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="12.75">
+    <row r="44" spans="1:8" ht="12.3">
       <c r="A44" s="4"/>
       <c r="F44" s="26">
         <f>B43-D43</f>
@@ -950,16 +953,16 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="12.75">
+    <row r="45" spans="1:8" ht="12.6">
       <c r="A45" s="27" t="str">
         <f>IF(AND(F43&gt;=0,F44&lt;=0), "Zero is contained in the interval so the difference is not statistically significant", "Zero is no longer contained in the interval so the difference is statistically significant")</f>
         <v>Zero is contained in the interval so the difference is not statistically significant</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="12.75">
+    <row r="46" spans="1:8" ht="12.3">
       <c r="C46" s="4"/>
     </row>
-    <row r="47" spans="1:8" ht="12.75">
+    <row r="47" spans="1:8" ht="12.3">
       <c r="A47" s="4" t="s">
         <v>33</v>
       </c>
@@ -985,7 +988,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="12.75">
+    <row r="48" spans="1:8" ht="12.3">
       <c r="F48" s="14">
         <f>B47-D47</f>
         <v>4.7191351181316565E-4</v>
@@ -994,13 +997,13 @@
         <v>34</v>
       </c>
     </row>
-    <row r="49" spans="1:1" ht="12.75">
+    <row r="49" spans="1:1" ht="12.6">
       <c r="A49" s="27" t="str">
-        <f>IF(AND(F47&gt;=0,F48&lt;=0), "Zero is contained in the interval so the difference is statistically significant", "Zero is no longer contained in the interval so the difference is statistically significant")</f>
+        <f>IF(AND(F47&gt;=0,F48&lt;=0), "Zero is contained in the interval so the difference is not statistically significant", "Zero is no longer contained in the interval so the difference is statistically significant")</f>
         <v>Zero is no longer contained in the interval so the difference is statistically significant</v>
       </c>
     </row>
-    <row r="53" spans="1:1" ht="12.75">
+    <row r="53" spans="1:1" ht="12.3">
       <c r="A53" s="28"/>
     </row>
   </sheetData>

</xml_diff>